<commit_message>
modify defaultScene and add png
+csv and xlsx
</commit_message>
<xml_diff>
--- a/Client/Resources/Data/Map/Map.xlsx
+++ b/Client/Resources/Data/Map/Map.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GA_6th_2Q_Project\GA_6th_2Q_Project\Client\Resources\Data\Map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ArcheTypeZero\GA_6th_2Q_Project\Client\Resources\Data\Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC19536-C3A5-4D92-9333-75BB62A65F2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E9C832-EAE4-4E86-9765-CBEE916B767B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -384,7 +384,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -443,352 +443,352 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
         <v>2</v>
       </c>
-      <c r="B7">
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
+      <c r="I7">
         <v>2</v>
       </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
       <c r="J7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
         <v>2</v>
       </c>
-      <c r="B8">
+      <c r="H8">
         <v>2</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
+      <c r="I8">
         <v>2</v>
       </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-      <c r="I8">
-        <v>3</v>
-      </c>
       <c r="J8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P8">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
         <v>2</v>
       </c>
-      <c r="B9">
+      <c r="H9">
         <v>2</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
+      <c r="I9">
         <v>2</v>
       </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
       <c r="J9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P9">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P10">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P11">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P12">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add Png and modify makeObject
</commit_message>
<xml_diff>
--- a/Client/Resources/Data/Map/Map.xlsx
+++ b/Client/Resources/Data/Map/Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ArcheTypeZero\GA_6th_2Q_Project\Client\Resources\Data\Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E9C832-EAE4-4E86-9765-CBEE916B767B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C356888-9336-458E-A1A8-58CF9D366ED7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -384,7 +384,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -443,352 +443,352 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P11">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>